<commit_message>
Configured listeners to write report and configured surefire plugin to run the maven test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\IdeaProjects\apiRelatime\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18851CA1-2194-49AE-81FB-7D1DF174D66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE0E17F-95EF-4281-8969-DCABD90D521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,7 +140,7 @@
     <t>test10@mailinator.com</t>
   </si>
   <si>
-    <t>cus_OehjJmR5GBWHrF</t>
+    <t>cus_RPYJT4w1QMVTp0</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added the customer Id to delete to trigger the build automatically from jenkins when pushed to github
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\IdeaProjects\apiRelatime\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE0E17F-95EF-4281-8969-DCABD90D521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C03CCA-2697-453A-8EFA-4545D92EF2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,7 +140,7 @@
     <t>test10@mailinator.com</t>
   </si>
   <si>
-    <t>cus_RPYJT4w1QMVTp0</t>
+    <t>cus_RPmLytin1swjzF</t>
   </si>
 </sst>
 </file>

</xml_diff>